<commit_message>
Added speed files for the modelica models
</commit_message>
<xml_diff>
--- a/data/boiler.xlsx
+++ b/data/boiler.xlsx
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>